<commit_message>
FS Mary Roth scoring test edits
</commit_message>
<xml_diff>
--- a/mary test data.xlsx
+++ b/mary test data.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760" tabRatio="500"/>
+    <workbookView xWindow="26700" yWindow="-80" windowWidth="35120" windowHeight="20280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +19,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+  <si>
+    <t>MR.L4.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L4.lesion.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L4.lesion.no</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L4.grazing.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L4.grazing.no</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L4.broken.tip</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>scan.id</t>
   </si>
@@ -39,93 +63,6 @@
     <t>no.leaves</t>
   </si>
   <si>
-    <t>sheath.length.cm</t>
-  </si>
-  <si>
-    <t>L1.length.cm</t>
-  </si>
-  <si>
-    <t>L1.area.cm2</t>
-  </si>
-  <si>
-    <t>L1.lesion.area.cm2</t>
-  </si>
-  <si>
-    <t>L1.lesion.no</t>
-  </si>
-  <si>
-    <t>L1.grazing.area.cm2</t>
-  </si>
-  <si>
-    <t>L1.grazing.no</t>
-  </si>
-  <si>
-    <t>L1.broken.tip</t>
-  </si>
-  <si>
-    <t>L2.length.cm</t>
-  </si>
-  <si>
-    <t>L2.area.cm2</t>
-  </si>
-  <si>
-    <t>L2.lesion.area.cm2</t>
-  </si>
-  <si>
-    <t>L2.lesion.no</t>
-  </si>
-  <si>
-    <t>L2.grazing.area.cm2</t>
-  </si>
-  <si>
-    <t>L2.grazing.no</t>
-  </si>
-  <si>
-    <t>L2.broken.tip</t>
-  </si>
-  <si>
-    <t>L3.length.cm</t>
-  </si>
-  <si>
-    <t>L3.area.cm2</t>
-  </si>
-  <si>
-    <t>L3.lesion.area.cm2</t>
-  </si>
-  <si>
-    <t>L3.lesion.no</t>
-  </si>
-  <si>
-    <t>L3.grazing.area.cm2</t>
-  </si>
-  <si>
-    <t>L3.grazing.no</t>
-  </si>
-  <si>
-    <t>L3.broken.tip</t>
-  </si>
-  <si>
-    <t>L4.length.cm</t>
-  </si>
-  <si>
-    <t>L4.area.cm2</t>
-  </si>
-  <si>
-    <t>L4.lesion.area.cm2</t>
-  </si>
-  <si>
-    <t>L4.lesion.no</t>
-  </si>
-  <si>
-    <t>L4.grazing.area.cm2</t>
-  </si>
-  <si>
-    <t>L4.grazing.no</t>
-  </si>
-  <si>
-    <t>L4.broken.tip</t>
-  </si>
-  <si>
     <t>scan.notes</t>
   </si>
   <si>
@@ -135,9 +72,6 @@
     <t>.</t>
   </si>
   <si>
-    <t>check</t>
-  </si>
-  <si>
     <t>L4 senescent</t>
   </si>
   <si>
@@ -148,13 +82,107 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>MR.L1.length.cm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L1.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L1.lesion.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L1.lesion.no</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L1.grazing.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L1.grazing.no</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L1.broken.tip</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L2.length.cm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L2.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L2.lesion.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L2.lesion.no</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L2.grazing.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L2.grazing.no</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L2.broken.tip</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L3.length.cm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L3.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L3.lesion.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L3.lesion.no</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L3.grazing.area.cm2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L3.grazing.no</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L3.broken.tip</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR.L4.length.cm</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,6 +208,10 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -198,25 +230,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -541,128 +569,162 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:32">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="AE1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32">
+      <c r="A2" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" t="s">
-        <v>25</v>
-      </c>
-      <c r="W1" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
+      <c r="C2">
+        <v>3.2959999999999998</v>
+      </c>
       <c r="D2">
-        <v>3.2959999999999998</v>
+        <v>1.1180000000000001</v>
       </c>
       <c r="E2">
-        <v>1.1180000000000001</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -673,102 +735,99 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2">
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2">
         <f>24.395+27.284</f>
         <v>51.679000000000002</v>
       </c>
-      <c r="L2">
+      <c r="K2">
         <f>10.44+9.544</f>
         <v>19.984000000000002</v>
       </c>
+      <c r="L2">
+        <v>1E-3</v>
+      </c>
       <c r="M2">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="N2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="O2">
         <v>1</v>
       </c>
-      <c r="O2">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2">
+      <c r="P2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2">
         <f>24.858+27.924+3.653+25.601</f>
         <v>82.036000000000001</v>
       </c>
-      <c r="S2">
+      <c r="R2">
         <f>11.61+1.486+10.253+10.154</f>
         <v>33.503</v>
       </c>
-      <c r="T2">
+      <c r="S2">
         <f>0.001+0.055+0.002</f>
         <v>5.8000000000000003E-2</v>
       </c>
+      <c r="T2">
+        <v>3</v>
+      </c>
       <c r="U2">
-        <v>3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="V2">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="W2">
         <v>1</v>
       </c>
+      <c r="W2" t="s">
+        <v>17</v>
+      </c>
       <c r="X2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="Y2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="Z2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="AA2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="AB2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="AC2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="AD2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="AE2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:32">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="C3">
         <f>25.283+11.969</f>
         <v>37.252000000000002</v>
       </c>
-      <c r="E3">
+      <c r="D3">
         <f>10.397+4.541</f>
         <v>14.938000000000001</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="F3">
         <v>0</v>
       </c>
@@ -778,212 +837,212 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3">
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3">
         <f>27.707+26.01+25.496+6.407</f>
         <v>85.61999999999999</v>
       </c>
-      <c r="L3">
+      <c r="K3">
         <f>2.424+10.372+10.881+11.54</f>
         <v>35.216999999999999</v>
       </c>
+      <c r="L3">
+        <v>5.0000000000000001E-3</v>
+      </c>
       <c r="M3">
-        <v>5.0000000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="N3">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="O3">
         <v>1</v>
       </c>
-      <c r="O3">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3">
+      <c r="P3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3">
         <f>25.743+26.915+18.251</f>
         <v>70.909000000000006</v>
       </c>
-      <c r="S3">
+      <c r="R3">
         <f>11.914+10.752+7.294</f>
         <v>29.96</v>
       </c>
-      <c r="T3">
+      <c r="S3">
         <f>0.043+0.015+0.002+0.009</f>
         <v>6.8999999999999992E-2</v>
       </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
       <c r="U3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V3">
         <v>0</v>
       </c>
-      <c r="W3">
-        <v>0</v>
-      </c>
-      <c r="X3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y3">
+      <c r="W3" t="s">
+        <v>18</v>
+      </c>
+      <c r="X3">
         <f>26.386+25.815+27.57</f>
         <v>79.771000000000001</v>
       </c>
-      <c r="Z3">
+      <c r="Y3">
         <f>10.297+10.608+11.029</f>
         <v>31.934000000000001</v>
       </c>
-      <c r="AA3">
+      <c r="Z3">
         <f>0.046+0.076+0.01+0.149+0.038+0.022+0.004+0.415+0.002+0.003+0.018+0.443+0.243+0.03+0.009</f>
         <v>1.5079999999999998</v>
       </c>
+      <c r="AA3">
+        <v>13</v>
+      </c>
       <c r="AB3">
-        <v>13</v>
-      </c>
-      <c r="AC3">
         <f>0.012+0.014+0.014+0.012</f>
         <v>5.2000000000000005E-2</v>
       </c>
-      <c r="AD3">
+      <c r="AC3">
         <v>4</v>
       </c>
+      <c r="AD3" t="s">
+        <v>17</v>
+      </c>
       <c r="AE3" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="AF3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:32">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
+      <c r="C4">
+        <v>8.5329999999999995</v>
+      </c>
       <c r="D4">
-        <v>8.5329999999999995</v>
+        <v>3.61</v>
       </c>
       <c r="E4">
-        <v>3.61</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="H4">
-        <v>2E-3</v>
-      </c>
-      <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K4">
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4">
         <f>25.861+26.075+8.333</f>
         <v>60.268999999999998</v>
       </c>
-      <c r="L4">
+      <c r="K4">
         <f>13.257+12.973+3.569</f>
         <v>29.798999999999999</v>
       </c>
-      <c r="M4">
+      <c r="L4">
         <f>0.052</f>
         <v>5.1999999999999998E-2</v>
       </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
       <c r="N4">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="O4">
         <v>1</v>
       </c>
-      <c r="O4">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>42</v>
-      </c>
-      <c r="R4">
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4">
         <f>25.943+27.061+26.663+12.287</f>
         <v>91.954000000000008</v>
       </c>
-      <c r="S4">
+      <c r="R4">
         <f>13.796+14.132+13.442+5.525</f>
         <v>46.894999999999996</v>
       </c>
-      <c r="T4">
+      <c r="S4">
         <f>0.008+0.011</f>
         <v>1.9E-2</v>
       </c>
+      <c r="T4">
+        <v>2</v>
+      </c>
       <c r="U4">
-        <v>2</v>
-      </c>
-      <c r="V4">
         <f>0.04</f>
         <v>0.04</v>
       </c>
-      <c r="W4">
+      <c r="V4">
         <v>1</v>
       </c>
-      <c r="X4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y4">
+      <c r="W4" t="s">
+        <v>18</v>
+      </c>
+      <c r="X4">
         <f>28.775+28.818+26.549+5.459</f>
         <v>89.600999999999999</v>
       </c>
-      <c r="Z4">
+      <c r="Y4">
         <f>27.472+15.202+2.19</f>
         <v>44.863999999999997</v>
       </c>
-      <c r="AA4">
+      <c r="Z4">
         <f>0.035+0.005+0.005+0.03+0.013+0.002+0.004+0.002+0.017</f>
         <v>0.113</v>
       </c>
+      <c r="AA4">
+        <v>9</v>
+      </c>
       <c r="AB4">
-        <v>9</v>
-      </c>
-      <c r="AC4">
         <f>0.005+0.015</f>
         <v>0.02</v>
       </c>
-      <c r="AD4">
+      <c r="AC4">
         <v>2</v>
       </c>
+      <c r="AD4" t="s">
+        <v>17</v>
+      </c>
       <c r="AE4" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="AF4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:32">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
+      <c r="C5">
+        <v>4.7309999999999999</v>
+      </c>
       <c r="D5">
-        <v>4.7309999999999999</v>
+        <v>1.73</v>
       </c>
       <c r="E5">
-        <v>1.73</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -994,97 +1053,94 @@
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>42</v>
-      </c>
-      <c r="K5">
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5">
         <f>25.303+20.993+7.43</f>
         <v>53.725999999999999</v>
       </c>
-      <c r="L5">
+      <c r="K5">
         <f>11.243+9.193+2.905</f>
         <v>23.341000000000001</v>
       </c>
+      <c r="L5">
+        <v>1E-3</v>
+      </c>
       <c r="M5">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="N5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="O5">
         <v>1</v>
       </c>
-      <c r="O5">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>42</v>
-      </c>
-      <c r="R5">
+      <c r="P5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q5">
         <f>25.501+25.512+24.653+7.125</f>
         <v>82.790999999999997</v>
       </c>
-      <c r="S5">
+      <c r="R5">
         <f>11.87+11.613+10.61+2.816</f>
         <v>36.908999999999999</v>
       </c>
-      <c r="T5">
+      <c r="S5">
         <f>0.008+0.01</f>
         <v>1.8000000000000002E-2</v>
       </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
       <c r="U5">
-        <v>2</v>
-      </c>
-      <c r="V5">
         <f>0.006+0.017+0.006+0.007</f>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="W5">
+      <c r="V5">
         <v>4</v>
       </c>
-      <c r="X5" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y5">
+      <c r="W5" t="s">
+        <v>18</v>
+      </c>
+      <c r="X5">
         <f>26.511+27.43+22.964+8.637</f>
         <v>85.542000000000002</v>
       </c>
-      <c r="Z5">
+      <c r="Y5">
         <f>11.823+12.063+9.397+3.374</f>
         <v>36.657000000000004</v>
       </c>
-      <c r="AA5">
+      <c r="Z5">
         <f>2.615+3.408+0.742+0.722+0.052+0.187+0.351+0.195+0.012+0.011+0.006+0.012+0.01+0.01+0.011+0.013+0.022+0.008+0.219+0.02+0.504</f>
         <v>9.1299999999999972</v>
       </c>
+      <c r="AA5">
+        <v>19</v>
+      </c>
       <c r="AB5">
-        <v>19</v>
-      </c>
-      <c r="AC5">
         <f>0.029+0.011</f>
         <v>0.04</v>
       </c>
-      <c r="AD5">
+      <c r="AC5">
         <v>2</v>
       </c>
+      <c r="AD5" t="s">
+        <v>17</v>
+      </c>
       <c r="AE5" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="AF5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>